<commit_message>
updated Login and Stack modules with get data from Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/DsAlgoTestData.xlsx
+++ b/src/test/resources/ExcelSheet/DsAlgoTestData.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2ac57a863a93e2b/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anand\eclipse-workspace\sample\DSALGO226BddFramework\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{367C5586-1034-4E5B-B803-6647F0D0B959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67997CB8-0BE8-49C6-9CA5-A15563A073B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDC8D4-907B-482D-AA4A-EBF21182E251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2988" yWindow="2100" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="testdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="sample" sheetId="2" r:id="rId2"/>
-    <sheet name="demo" sheetId="3" r:id="rId3"/>
+    <sheet name="phythonTryEditor" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Tetscases</t>
   </si>
@@ -34,13 +34,125 @@
   </si>
   <si>
     <t>print(5+8)</t>
+  </si>
+  <si>
+    <t>testId</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>invalid@test.com</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>TestNinja</t>
+  </si>
+  <si>
+    <t>C5Mha6FkdSAVEN@</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Valid Input</t>
+  </si>
+  <si>
+    <t>Invalid Input</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <r>
+      <t>print(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"hello"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>print hello</t>
+  </si>
+  <si>
+    <t>print '5+10</t>
+  </si>
+  <si>
+    <t>Tc002</t>
+  </si>
+  <si>
+    <r>
+      <t>print(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -52,6 +164,48 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,14 +225,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -92,10 +253,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -299,57 +456,147 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{14EC9537-1E9E-43B0-A7F6-DAFB39369405}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703CB7AA-E2A6-4D23-8607-DF0540B8BB06}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB62542F-A62F-4391-A8C2-FCDE11742EDC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Excel data for LinkedList & Queue
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/DsAlgoTestData.xlsx
+++ b/src/test/resources/ExcelSheet/DsAlgoTestData.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2ac57a863a93e2b/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{367C5586-1034-4E5B-B803-6647F0D0B959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67997CB8-0BE8-49C6-9CA5-A15563A073B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8DD7B76D-75EB-4118-BB80-B8809887F949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +13,12 @@
     <sheet name="demo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Tetscases</t>
   </si>
@@ -34,6 +30,18 @@
   </si>
   <si>
     <t>print(5+8)</t>
+  </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>print(5*8)</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>print(15-8)</t>
   </si>
 </sst>
 </file>
@@ -92,10 +100,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -299,10 +303,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -321,6 +325,22 @@
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Home Login and Register Modules
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/DsAlgoTestData.xlsx
+++ b/src/test/resources/ExcelSheet/DsAlgoTestData.xlsx
@@ -3,23 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3E550D5C-5F9C-48B2-B615-72569DFBF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{10109174-51F0-4166-91A4-E1C8DBD8EF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19400" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="4" r:id="rId1"/>
     <sheet name="Login" sheetId="1" r:id="rId2"/>
-    <sheet name="sample" sheetId="2" r:id="rId3"/>
-    <sheet name="phythonTryEditor" sheetId="3" r:id="rId4"/>
+    <sheet name="Register" sheetId="5" r:id="rId3"/>
+    <sheet name="sample" sheetId="2" r:id="rId4"/>
+    <sheet name="phythonTryEditor" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R16"/>
+  <oleSize ref="A1:E19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>Tetscases</t>
   </si>
@@ -52,12 +53,6 @@
   </si>
   <si>
     <t>C5Mha6FkdSAVEN@</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
   </si>
   <si>
     <t>Stack</t>
@@ -99,9 +94,6 @@
   </si>
   <si>
     <t>print '5+10</t>
-  </si>
-  <si>
-    <t>Tc002</t>
   </si>
   <si>
     <r>
@@ -148,17 +140,90 @@
     <t>ArrayList</t>
   </si>
   <si>
+    <t>print(5*8)</t>
+  </si>
+  <si>
     <t>Graph</t>
   </si>
   <si>
-    <t>StackList</t>
+    <t>print(15-8)</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please fill out this field </t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>Testuser</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>C5Mha6FkdSAVEN@1234</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>New Account Created.</t>
+  </si>
+  <si>
+    <t>user_name946b36d6</t>
+  </si>
+  <si>
+    <t>user_name73a0d16d</t>
+  </si>
+  <si>
+    <t>user_name6f6aa073</t>
+  </si>
+  <si>
+    <t>user_name7084d229</t>
+  </si>
+  <si>
+    <t>user_name1f9acbf2</t>
+  </si>
+  <si>
+    <t>user_name5958e797</t>
+  </si>
+  <si>
+    <t>user_name0f846a02</t>
+  </si>
+  <si>
+    <t>user_name9bfcbabf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -213,6 +278,20 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF004085"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -235,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -243,6 +322,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -459,48 +540,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795A697F-9D83-44EA-AB3D-D3C85043ABBA}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -511,19 +590,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="20.88671875"/>
+    <col min="3" max="3" customWidth="true" width="20.44140625"/>
+    <col min="4" max="4" customWidth="true" width="30.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -533,68 +613,260 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{14EC9537-1E9E-43B0-A7F6-DAFB39369405}"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{14EC9537-1E9E-43B0-A7F6-DAFB39369405}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E410F791-E237-43A3-B589-5F695EDB9C9B}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="21.5546875"/>
+    <col min="3" max="3" customWidth="true" width="20.33203125"/>
+    <col min="4" max="4" customWidth="true" width="30.6640625"/>
+    <col min="5" max="5" customWidth="true" width="56.109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1" xr:uid="{9FD03C6F-9C51-43EF-8A1B-B8DE37C867E3}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{3E991483-47D3-4216-8F99-1B7840174B8B}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{A37E425C-A42C-4300-8351-512384EDBA46}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703CB7AA-E2A6-4D23-8607-DF0540B8BB06}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.109375"/>
+    <col min="2" max="2" customWidth="true" width="15.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -602,53 +874,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB62542F-A62F-4391-A8C2-FCDE11742EDC}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.5546875"/>
+    <col min="2" max="2" customWidth="true" style="4" width="17.6640625"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>17</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>